<commit_message>
update excel effort estimation
</commit_message>
<xml_diff>
--- a/doc/Effort_Estimation/DAGoPERT_2016_slim.xlsx
+++ b/doc/Effort_Estimation/DAGoPERT_2016_slim.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr codeName="DieseArbeitsmappe"/>
   <bookViews>
-    <workbookView windowWidth="30720" windowHeight="13655" tabRatio="758" activeTab="1"/>
+    <workbookView windowWidth="30720" windowHeight="13655" tabRatio="758" firstSheet="1" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Info" sheetId="18" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="186" uniqueCount="103">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="192" uniqueCount="109">
   <si>
     <t>Delphi Verfahren mit PERT - Unsicherheit ausdrückbar durch Schätzbereich: Breite, p(range)</t>
   </si>
@@ -105,16 +105,34 @@
     <t>Team develops mockup to visualize interface which will be in use at PresentationLab and live demonstration</t>
   </si>
   <si>
+    <t>choose collaboration tool to create mockups</t>
+  </si>
+  <si>
+    <t>create 2 mockups to display user interface</t>
+  </si>
+  <si>
     <t>3D print</t>
   </si>
   <si>
     <t>Finally supporting equipment for raspberry pi will be created via 3D print at ProjectKitchen</t>
   </si>
   <si>
+    <t>request date and time to visit ProjectKitchen for 3D print</t>
+  </si>
+  <si>
     <t>Software final development</t>
   </si>
   <si>
     <t>Software gets final design and bugfixes</t>
+  </si>
+  <si>
+    <t>browses alternative recognition software for handling out/in scope</t>
+  </si>
+  <si>
+    <t>discussion with supervisor about specified requirement of daily/current counter</t>
+  </si>
+  <si>
+    <t>adapt software to recognize people on whole body or bodyparts only</t>
   </si>
   <si>
     <t>Connect Hardware + Software</t>
@@ -412,15 +430,15 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="7">
-    <numFmt numFmtId="176" formatCode="0.0"/>
+    <numFmt numFmtId="176" formatCode="&quot;€&quot;\ #,##0.00;[Red]\-&quot;€&quot;\ #,##0.00"/>
+    <numFmt numFmtId="41" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
+    <numFmt numFmtId="43" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
     <numFmt numFmtId="177" formatCode="_-&quot;€&quot;\ * #,##0_-;\-&quot;€&quot;\ * #,##0_-;_-&quot;€&quot;\ * \-_-;_-@_-"/>
-    <numFmt numFmtId="43" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
-    <numFmt numFmtId="41" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
     <numFmt numFmtId="178" formatCode="_-&quot;€&quot;\ * #,##0.00_-;\-&quot;€&quot;\ * #,##0.00_-;_-&quot;€&quot;\ * \-??_-;_-@_-"/>
-    <numFmt numFmtId="179" formatCode="&quot;€&quot;\ #,##0.00;[Red]\-&quot;€&quot;\ #,##0.00"/>
+    <numFmt numFmtId="179" formatCode="0.0"/>
     <numFmt numFmtId="180" formatCode="0.000"/>
   </numFmts>
-  <fonts count="33">
+  <fonts count="31">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -443,11 +461,6 @@
     </font>
     <font>
       <b/>
-      <sz val="10"/>
-      <name val="Arial"/>
-      <charset val="134"/>
-    </font>
-    <font>
       <sz val="10"/>
       <name val="Arial"/>
       <charset val="134"/>
@@ -498,6 +511,51 @@
       <charset val="134"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="15"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <b/>
       <sz val="11"/>
       <color rgb="FF3F3F3F"/>
@@ -507,21 +565,7 @@
     </font>
     <font>
       <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
+      <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -536,7 +580,7 @@
     </font>
     <font>
       <sz val="11"/>
-      <color theme="0"/>
+      <color rgb="FF9C0006"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -566,13 +610,6 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <b/>
       <sz val="18"/>
       <color theme="3"/>
@@ -586,22 +623,6 @@
       <color rgb="FF7F7F7F"/>
       <name val="Calibri"/>
       <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="15"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -619,16 +640,8 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
       <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
+      <color rgb="FF9C6500"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -636,14 +649,7 @@
     <font>
       <b/>
       <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
+      <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -683,7 +689,49 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -695,31 +743,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -731,25 +755,19 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="6" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
+        <fgColor theme="5" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
+        <fgColor theme="5" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -773,25 +791,19 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="4" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
+        <fgColor theme="9" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -803,13 +815,25 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="4"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5"/>
+        <fgColor theme="4" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -821,25 +845,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
+        <fgColor theme="5"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1347,32 +1353,22 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF3F3F3F"/>
-      </right>
+      <left/>
+      <right/>
       <top style="thin">
-        <color rgb="FF3F3F3F"/>
+        <color theme="4"/>
       </top>
-      <bottom style="thin">
-        <color rgb="FF3F3F3F"/>
+      <bottom style="double">
+        <color theme="4"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
-      <left style="double">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="double">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="double">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="double">
-        <color rgb="FF3F3F3F"/>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
       </bottom>
       <diagonal/>
     </border>
@@ -1401,11 +1397,41 @@
       <diagonal/>
     </border>
     <border>
+      <left style="thin">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
       <left/>
       <right/>
       <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="double">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="double">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="double">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="double">
+        <color rgb="FF3F3F3F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -1424,186 +1450,166 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
-      <bottom style="double">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="62">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="15" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="43" fontId="13" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="43" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="41" fontId="13" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="41" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
-    <xf numFmtId="177" fontId="13" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="177" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="178" fontId="13" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="178" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="9" fontId="13" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="9" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="17" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="12" borderId="40" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="41" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="13" borderId="42" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="13" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="22" fillId="15" borderId="45" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="41" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="2" fillId="9" borderId="42" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="41" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="43" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="26" fillId="17" borderId="44" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="41" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="40" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="27" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="5" borderId="39" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="26" fillId="19" borderId="46" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="13" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="28" fillId="5" borderId="44" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="27" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="29" fillId="0" borderId="45" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="17" fillId="11" borderId="43" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="30" fillId="0" borderId="46" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="29" fillId="11" borderId="46" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="31" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="44" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="39" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="15" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="20" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="28" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="13" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="11" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="15" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="13" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="13" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="11" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="13" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="13" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="13" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="13" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="17" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="13" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="13" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="13" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="173">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
@@ -1638,23 +1644,23 @@
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="179" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyProtection="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyProtection="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyProtection="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyProtection="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="1" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="1" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center"/>
       <protection locked="0"/>
     </xf>
@@ -1666,10 +1672,10 @@
     <xf numFmtId="1" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="49" fontId="4" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="176" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="179" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyProtection="1"/>
@@ -1711,14 +1717,14 @@
     <xf numFmtId="2" fontId="3" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center"/>
       <protection locked="0"/>
     </xf>
     <xf numFmtId="2" fontId="3" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center"/>
       <protection locked="0"/>
     </xf>
@@ -1731,7 +1737,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -1753,19 +1759,19 @@
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="2" fontId="6" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyProtection="1">
+    <xf numFmtId="2" fontId="5" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyProtection="1">
       <protection locked="0"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="2" fontId="6" fillId="0" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyProtection="1">
+    <xf numFmtId="2" fontId="5" fillId="0" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyProtection="1">
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="2" fontId="8" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -1780,24 +1786,24 @@
     </xf>
     <xf numFmtId="2" fontId="3" fillId="0" borderId="20" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="2" fontId="3" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="2" fontId="4" fillId="0" borderId="20" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="2" fontId="4" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="179" fontId="4" fillId="0" borderId="20" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="179" fontId="4" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="179" fontId="3" fillId="0" borderId="20" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="2" fontId="4" fillId="0" borderId="20" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="2" fontId="4" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="179" fontId="3" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="49" fontId="8" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="20" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="176" fontId="0" fillId="0" borderId="20" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="176" fontId="0" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="176" fontId="3" fillId="0" borderId="20" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="20" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="176" fontId="3" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="7" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="8" fillId="0" borderId="21" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="7" fillId="0" borderId="21" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="8" fillId="0" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="7" fillId="0" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="3" fontId="8" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="3" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1805,22 +1811,22 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyProtection="1">
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="2" fontId="3" fillId="0" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -1836,10 +1842,10 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="9" fontId="4" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="2" fontId="4" fillId="0" borderId="20" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="20" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="20" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
@@ -1869,15 +1875,15 @@
     <xf numFmtId="2" fontId="3" fillId="2" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="1">
       <alignment vertical="top" wrapText="1"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="9" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="49" fontId="3" fillId="0" borderId="26" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
@@ -1892,7 +1898,7 @@
       <alignment vertical="top" wrapText="1"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="179" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
       <protection locked="0"/>
     </xf>
@@ -1925,45 +1931,45 @@
       <alignment vertical="top" wrapText="1"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="31" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="31" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="49" fontId="10" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="49" fontId="9" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="32" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="32" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="176" fontId="10" fillId="0" borderId="33" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="179" fontId="9" fillId="0" borderId="33" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="176" fontId="10" fillId="0" borderId="32" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="179" fontId="9" fillId="0" borderId="32" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="34" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="34" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="11" fillId="4" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="49" fontId="10" fillId="4" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="2" fontId="11" fillId="4" borderId="20" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="2" fontId="10" fillId="4" borderId="20" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="176" fontId="11" fillId="4" borderId="35" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="179" fontId="10" fillId="4" borderId="35" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="176" fontId="11" fillId="4" borderId="20" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="179" fontId="10" fillId="4" borderId="20" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="2" fontId="11" fillId="4" borderId="36" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="2" fontId="10" fillId="4" borderId="36" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="4" fillId="0" borderId="26" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="26" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
       <protection locked="0"/>
     </xf>
@@ -1971,23 +1977,23 @@
       <alignment horizontal="center" vertical="top" wrapText="1"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="49" fontId="8" fillId="0" borderId="26" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="49" fontId="7" fillId="0" borderId="26" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment vertical="top" wrapText="1"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment vertical="top" wrapText="1"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment wrapText="1"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="176" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="179" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
       <protection locked="0"/>
     </xf>
@@ -1999,47 +2005,47 @@
       <alignment horizontal="center" vertical="top" wrapText="1"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="2" fontId="10" fillId="4" borderId="32" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="2" fontId="9" fillId="4" borderId="32" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="2" fontId="10" fillId="4" borderId="34" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="2" fontId="9" fillId="4" borderId="34" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="2" fontId="10" fillId="3" borderId="32" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="2" fontId="9" fillId="3" borderId="32" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="180" fontId="10" fillId="4" borderId="33" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="180" fontId="9" fillId="4" borderId="33" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="4" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="9" fillId="4" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="4" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="9" fillId="4" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="37" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="37" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="2" fontId="11" fillId="4" borderId="20" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="2" fontId="10" fillId="4" borderId="20" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="2" fontId="11" fillId="4" borderId="36" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="2" fontId="10" fillId="4" borderId="36" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="180" fontId="11" fillId="4" borderId="35" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="180" fontId="10" fillId="4" borderId="35" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="180" fontId="11" fillId="4" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="180" fontId="10" fillId="4" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="2" fontId="11" fillId="4" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="2" fontId="10" fillId="4" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="2" fontId="11" fillId="4" borderId="38" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="2" fontId="10" fillId="4" borderId="38" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="180" fontId="0" fillId="4" borderId="5" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
@@ -2052,7 +2058,7 @@
       <alignment horizontal="center" vertical="top" wrapText="1"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="2" fontId="11" fillId="4" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="2" fontId="10" fillId="4" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
@@ -2252,49 +2258,49 @@
                 <c:formatCode>0.00</c:formatCode>
                 <c:ptCount val="15"/>
                 <c:pt idx="0">
-                  <c:v>0</c:v>
+                  <c:v>0.0660593695372309</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0</c:v>
+                  <c:v>0.0700279965038278</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0</c:v>
+                  <c:v>0.0715713514352821</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0</c:v>
+                  <c:v>0.0724532685389703</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0</c:v>
+                  <c:v>0.073390305461639</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0</c:v>
+                  <c:v>0.0742171027463467</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>0</c:v>
+                  <c:v>0.0757053378588205</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>0</c:v>
+                  <c:v>0.0770833333333333</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>0</c:v>
+                  <c:v>0.0784613288078461</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>0</c:v>
+                  <c:v>0.07994956392032</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>0</c:v>
+                  <c:v>0.0807763612050277</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>0</c:v>
+                  <c:v>0.0817133981276964</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>0</c:v>
+                  <c:v>0.0825953152313846</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>0</c:v>
+                  <c:v>0.0841386701628389</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>0</c:v>
+                  <c:v>0.0881072971294358</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3583,8 +3589,8 @@
   </sheetPr>
   <dimension ref="A1:Q358"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="C10" sqref="C10"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="P4" sqref="P4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.4259259259259" defaultRowHeight="13.2"/>
@@ -3692,34 +3698,34 @@
       <c r="D3" s="140"/>
       <c r="E3" s="141">
         <f>SUM(E4:E10001)</f>
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="F3" s="142">
         <f>SUM(F4:F10001)</f>
-        <v>0</v>
+        <v>12</v>
       </c>
       <c r="G3" s="142">
         <f>SUM(G4:G10001)</f>
-        <v>0</v>
+        <v>18</v>
       </c>
       <c r="H3" s="143"/>
       <c r="I3" s="161">
         <f>SUM(I4:I10001)</f>
-        <v>0</v>
+        <v>12.3333333333333</v>
       </c>
       <c r="J3" s="162">
         <f>SUM(J4:J10001)</f>
-        <v>0</v>
+        <v>12.3333333333333</v>
       </c>
       <c r="K3" s="161"/>
       <c r="L3" s="161"/>
       <c r="M3" s="163">
         <f>N3^(1/2)</f>
-        <v>0</v>
+        <v>0.881917103688197</v>
       </c>
       <c r="N3" s="164">
         <f>SUM(N4:N10001)</f>
-        <v>0</v>
+        <v>0.777777777777778</v>
       </c>
       <c r="O3" s="165"/>
       <c r="P3" s="166"/>
@@ -3769,24 +3775,27 @@
         <v/>
       </c>
     </row>
-    <row r="5" ht="39.6" spans="1:17">
+    <row r="5" ht="26.4" spans="1:17">
       <c r="A5" s="146"/>
-      <c r="B5" s="121" t="s">
+      <c r="D5" s="121" t="s">
         <v>21</v>
       </c>
-      <c r="C5" s="121" t="s">
-        <v>22</v>
-      </c>
-      <c r="E5" s="145"/>
-      <c r="F5" s="145"/>
-      <c r="G5" s="145"/>
-      <c r="I5" s="123" t="str">
+      <c r="E5" s="145">
+        <v>1</v>
+      </c>
+      <c r="F5" s="145">
+        <v>1</v>
+      </c>
+      <c r="G5" s="145">
+        <v>2</v>
+      </c>
+      <c r="I5" s="123">
         <f>IF(OR(E5="",F5="",G5=""),"",(E5+(4*F5)+G5)/6)</f>
-        <v/>
-      </c>
-      <c r="J5" s="124" t="str">
+        <v>1.16666666666667</v>
+      </c>
+      <c r="J5" s="124">
         <f t="shared" ref="J5:J68" si="5">IF(I5="","",I5*storypoints_kalibrierung)</f>
-        <v/>
+        <v>1.16666666666667</v>
       </c>
       <c r="K5" s="125">
         <v>99.73</v>
@@ -3795,17 +3804,17 @@
         <f t="shared" ref="L5:L32" si="6">INDEX(prozentsatz_divisor,(MATCH(K5,prozentsatz_divisor_prozent,-1)+1),2)</f>
         <v>6</v>
       </c>
-      <c r="M5" s="127" t="str">
+      <c r="M5" s="127">
         <f>IF(I5="","",((G5-E5)/L5)*storypoints_kalibrierung)</f>
-        <v/>
-      </c>
-      <c r="N5" s="167" t="str">
+        <v>0.166666666666667</v>
+      </c>
+      <c r="N5" s="167">
         <f t="shared" ref="N5:N68" si="7">IF(I5="","",M5^2)</f>
-        <v/>
+        <v>0.0277777777777778</v>
       </c>
       <c r="O5" s="168" t="str">
         <f t="shared" si="3"/>
-        <v/>
+        <v>S</v>
       </c>
       <c r="P5" s="169"/>
       <c r="Q5" s="171" t="str">
@@ -3813,24 +3822,27 @@
         <v/>
       </c>
     </row>
-    <row r="6" ht="26.4" spans="1:17">
+    <row r="6" spans="1:17">
       <c r="A6" s="144"/>
-      <c r="B6" s="147" t="s">
-        <v>23</v>
-      </c>
-      <c r="C6" s="147" t="s">
-        <v>24</v>
-      </c>
-      <c r="E6" s="145"/>
-      <c r="F6" s="145"/>
-      <c r="G6" s="145"/>
-      <c r="I6" s="123" t="str">
+      <c r="D6" s="121" t="s">
+        <v>22</v>
+      </c>
+      <c r="E6" s="145">
+        <v>2</v>
+      </c>
+      <c r="F6" s="145">
+        <v>2</v>
+      </c>
+      <c r="G6" s="145">
+        <v>3</v>
+      </c>
+      <c r="I6" s="123">
         <f t="shared" ref="I6:I68" si="9">IF(OR(E6="",F6="",G6=""),"",(E6+(4*F6)+G6)/6)</f>
-        <v/>
-      </c>
-      <c r="J6" s="124" t="str">
+        <v>2.16666666666667</v>
+      </c>
+      <c r="J6" s="124">
         <f t="shared" si="5"/>
-        <v/>
+        <v>2.16666666666667</v>
       </c>
       <c r="K6" s="125">
         <v>99.73</v>
@@ -3839,17 +3851,17 @@
         <f t="shared" si="6"/>
         <v>6</v>
       </c>
-      <c r="M6" s="127" t="str">
+      <c r="M6" s="127">
         <f t="shared" ref="M6:M68" si="10">IF(I6="","",((G6-E6)/L6)*storypoints_kalibrierung)</f>
-        <v/>
-      </c>
-      <c r="N6" s="167" t="str">
+        <v>0.166666666666667</v>
+      </c>
+      <c r="N6" s="167">
         <f t="shared" si="7"/>
-        <v/>
+        <v>0.0277777777777778</v>
       </c>
       <c r="O6" s="168" t="str">
         <f t="shared" si="3"/>
-        <v/>
+        <v>M</v>
       </c>
       <c r="P6" s="169"/>
       <c r="Q6" s="171" t="str">
@@ -3857,13 +3869,13 @@
         <v/>
       </c>
     </row>
-    <row r="7" ht="52.8" spans="1:17">
+    <row r="7" ht="39.6" spans="1:17">
       <c r="A7" s="144"/>
-      <c r="B7" s="147" t="s">
-        <v>25</v>
-      </c>
-      <c r="C7" s="147" t="s">
-        <v>26</v>
+      <c r="B7" s="121" t="s">
+        <v>23</v>
+      </c>
+      <c r="C7" s="121" t="s">
+        <v>24</v>
       </c>
       <c r="E7" s="145"/>
       <c r="F7" s="145"/>
@@ -3901,24 +3913,27 @@
         <v/>
       </c>
     </row>
-    <row r="8" ht="39.6" spans="1:17">
+    <row r="8" ht="26.4" spans="1:17">
       <c r="A8" s="144"/>
-      <c r="B8" s="147" t="s">
-        <v>27</v>
-      </c>
-      <c r="C8" s="147" t="s">
-        <v>28</v>
-      </c>
-      <c r="E8" s="145"/>
-      <c r="F8" s="145"/>
-      <c r="G8" s="145"/>
-      <c r="I8" s="123" t="str">
+      <c r="D8" s="121" t="s">
+        <v>25</v>
+      </c>
+      <c r="E8" s="145">
+        <v>1</v>
+      </c>
+      <c r="F8" s="145">
+        <v>1</v>
+      </c>
+      <c r="G8" s="145">
+        <v>2</v>
+      </c>
+      <c r="I8" s="123">
         <f t="shared" si="9"/>
-        <v/>
-      </c>
-      <c r="J8" s="124" t="str">
+        <v>1.16666666666667</v>
+      </c>
+      <c r="J8" s="124">
         <f t="shared" si="5"/>
-        <v/>
+        <v>1.16666666666667</v>
       </c>
       <c r="K8" s="125">
         <v>99.73</v>
@@ -3927,17 +3942,17 @@
         <f t="shared" si="6"/>
         <v>6</v>
       </c>
-      <c r="M8" s="127" t="str">
+      <c r="M8" s="127">
         <f t="shared" si="10"/>
-        <v/>
-      </c>
-      <c r="N8" s="167" t="str">
+        <v>0.166666666666667</v>
+      </c>
+      <c r="N8" s="167">
         <f t="shared" si="7"/>
-        <v/>
+        <v>0.0277777777777778</v>
       </c>
       <c r="O8" s="168" t="str">
         <f t="shared" si="3"/>
-        <v/>
+        <v>S</v>
       </c>
       <c r="P8" s="169"/>
       <c r="Q8" s="171" t="str">
@@ -3945,13 +3960,13 @@
         <v/>
       </c>
     </row>
-    <row r="9" ht="39.6" spans="1:17">
+    <row r="9" ht="26.4" spans="1:17">
       <c r="A9" s="144"/>
       <c r="B9" s="147" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="C9" s="147" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="E9" s="145"/>
       <c r="F9" s="145"/>
@@ -3989,19 +4004,27 @@
         <v/>
       </c>
     </row>
-    <row r="10" spans="1:17">
+    <row r="10" ht="26.4" spans="1:17">
       <c r="A10" s="144"/>
-      <c r="B10" s="121"/>
-      <c r="E10" s="145"/>
-      <c r="F10" s="145"/>
-      <c r="G10" s="145"/>
-      <c r="I10" s="123" t="str">
+      <c r="D10" s="121" t="s">
+        <v>28</v>
+      </c>
+      <c r="E10" s="145">
+        <v>1</v>
+      </c>
+      <c r="F10" s="145">
+        <v>3</v>
+      </c>
+      <c r="G10" s="145">
+        <v>5</v>
+      </c>
+      <c r="I10" s="123">
         <f t="shared" si="9"/>
-        <v/>
-      </c>
-      <c r="J10" s="124" t="str">
+        <v>3</v>
+      </c>
+      <c r="J10" s="124">
         <f t="shared" si="5"/>
-        <v/>
+        <v>3</v>
       </c>
       <c r="K10" s="125">
         <v>99.73</v>
@@ -4010,17 +4033,17 @@
         <f t="shared" si="6"/>
         <v>6</v>
       </c>
-      <c r="M10" s="127" t="str">
+      <c r="M10" s="127">
         <f t="shared" si="10"/>
-        <v/>
-      </c>
-      <c r="N10" s="167" t="str">
+        <v>0.666666666666667</v>
+      </c>
+      <c r="N10" s="167">
         <f t="shared" si="7"/>
-        <v/>
+        <v>0.444444444444444</v>
       </c>
       <c r="O10" s="168" t="str">
         <f t="shared" si="3"/>
-        <v/>
+        <v>M</v>
       </c>
       <c r="P10" s="169"/>
       <c r="Q10" s="171" t="str">
@@ -4028,20 +4051,27 @@
         <v/>
       </c>
     </row>
-    <row r="11" spans="1:17">
+    <row r="11" ht="26.4" spans="1:17">
       <c r="A11" s="144"/>
-      <c r="B11" s="148"/>
-      <c r="C11" s="147"/>
-      <c r="E11" s="145"/>
-      <c r="F11" s="145"/>
-      <c r="G11" s="145"/>
-      <c r="I11" s="123" t="str">
+      <c r="D11" s="121" t="s">
+        <v>29</v>
+      </c>
+      <c r="E11" s="145">
+        <v>1</v>
+      </c>
+      <c r="F11" s="145">
+        <v>1</v>
+      </c>
+      <c r="G11" s="145">
+        <v>1</v>
+      </c>
+      <c r="I11" s="123">
         <f t="shared" si="9"/>
-        <v/>
-      </c>
-      <c r="J11" s="124" t="str">
+        <v>1</v>
+      </c>
+      <c r="J11" s="124">
         <f t="shared" si="5"/>
-        <v/>
+        <v>1</v>
       </c>
       <c r="K11" s="125">
         <v>99.73</v>
@@ -4050,17 +4080,17 @@
         <f t="shared" si="6"/>
         <v>6</v>
       </c>
-      <c r="M11" s="127" t="str">
+      <c r="M11" s="127">
         <f t="shared" si="10"/>
-        <v/>
-      </c>
-      <c r="N11" s="167" t="str">
+        <v>0</v>
+      </c>
+      <c r="N11" s="167">
         <f t="shared" si="7"/>
-        <v/>
+        <v>0</v>
       </c>
       <c r="O11" s="168" t="str">
         <f t="shared" si="3"/>
-        <v/>
+        <v>S</v>
       </c>
       <c r="P11" s="169"/>
       <c r="Q11" s="171" t="str">
@@ -4068,19 +4098,27 @@
         <v/>
       </c>
     </row>
-    <row r="12" spans="1:17">
+    <row r="12" ht="26.4" spans="1:17">
       <c r="A12" s="144"/>
-      <c r="B12" s="148"/>
-      <c r="E12" s="145"/>
-      <c r="F12" s="145"/>
-      <c r="G12" s="145"/>
-      <c r="I12" s="123" t="str">
+      <c r="D12" s="121" t="s">
+        <v>30</v>
+      </c>
+      <c r="E12" s="145">
+        <v>2</v>
+      </c>
+      <c r="F12" s="145">
+        <v>4</v>
+      </c>
+      <c r="G12" s="145">
+        <v>5</v>
+      </c>
+      <c r="I12" s="123">
         <f t="shared" si="9"/>
-        <v/>
-      </c>
-      <c r="J12" s="124" t="str">
+        <v>3.83333333333333</v>
+      </c>
+      <c r="J12" s="124">
         <f t="shared" si="5"/>
-        <v/>
+        <v>3.83333333333333</v>
       </c>
       <c r="K12" s="125">
         <v>99.73</v>
@@ -4089,17 +4127,17 @@
         <f t="shared" si="6"/>
         <v>6</v>
       </c>
-      <c r="M12" s="127" t="str">
+      <c r="M12" s="127">
         <f t="shared" si="10"/>
-        <v/>
-      </c>
-      <c r="N12" s="167" t="str">
+        <v>0.5</v>
+      </c>
+      <c r="N12" s="167">
         <f t="shared" si="7"/>
-        <v/>
+        <v>0.25</v>
       </c>
       <c r="O12" s="168" t="str">
         <f t="shared" si="3"/>
-        <v/>
+        <v>M</v>
       </c>
       <c r="P12" s="169"/>
       <c r="Q12" s="171" t="str">
@@ -4107,9 +4145,14 @@
         <v/>
       </c>
     </row>
-    <row r="13" spans="1:17">
+    <row r="13" ht="52.8" spans="1:17">
       <c r="A13" s="144"/>
-      <c r="B13" s="148"/>
+      <c r="B13" s="147" t="s">
+        <v>31</v>
+      </c>
+      <c r="C13" s="147" t="s">
+        <v>32</v>
+      </c>
       <c r="E13" s="145"/>
       <c r="F13" s="145"/>
       <c r="G13" s="145"/>
@@ -4146,9 +4189,14 @@
         <v/>
       </c>
     </row>
-    <row r="14" spans="1:17">
+    <row r="14" ht="39.6" spans="1:17">
       <c r="A14" s="144"/>
-      <c r="B14" s="148"/>
+      <c r="B14" s="147" t="s">
+        <v>33</v>
+      </c>
+      <c r="C14" s="147" t="s">
+        <v>34</v>
+      </c>
       <c r="E14" s="145"/>
       <c r="F14" s="145"/>
       <c r="G14" s="145"/>
@@ -4185,9 +4233,14 @@
         <v/>
       </c>
     </row>
-    <row r="15" spans="1:17">
+    <row r="15" ht="39.6" spans="1:17">
       <c r="A15" s="146"/>
-      <c r="B15" s="148"/>
+      <c r="B15" s="147" t="s">
+        <v>35</v>
+      </c>
+      <c r="C15" s="147" t="s">
+        <v>36</v>
+      </c>
       <c r="E15" s="145"/>
       <c r="F15" s="145"/>
       <c r="G15" s="145"/>
@@ -15230,7 +15283,7 @@
   <sheetData>
     <row r="1" spans="1:11">
       <c r="A1" s="94" t="s">
-        <v>31</v>
+        <v>37</v>
       </c>
       <c r="B1" s="95"/>
       <c r="C1" s="95"/>
@@ -15249,19 +15302,19 @@
     </row>
     <row r="3" s="54" customFormat="1" ht="30.75" customHeight="1" spans="1:10">
       <c r="A3" s="100" t="s">
-        <v>32</v>
+        <v>38</v>
       </c>
       <c r="B3" s="101" t="s">
-        <v>33</v>
+        <v>39</v>
       </c>
       <c r="C3" s="101" t="s">
-        <v>34</v>
+        <v>40</v>
       </c>
       <c r="D3" s="101" t="s">
-        <v>35</v>
+        <v>41</v>
       </c>
       <c r="E3" s="102" t="s">
-        <v>36</v>
+        <v>42</v>
       </c>
       <c r="G3" s="103"/>
       <c r="H3" s="103"/>
@@ -15274,19 +15327,19 @@
       </c>
       <c r="B4" s="105">
         <f>IF((Spezifikation!J3-(2*Spezifikation!M3))&lt;0,"NV",(Spezifikation!J3-(2*Spezifikation!M3)))</f>
-        <v>0</v>
+        <v>10.5694991259569</v>
       </c>
       <c r="C4" s="106">
         <f>IF(B4="NV",C5,B4/Einstellungen!$B$53)</f>
-        <v>0</v>
+        <v>1.32118739074462</v>
       </c>
       <c r="D4" s="106">
         <f>IF(B4="NV",D5,B4/Einstellungen!$B$54)</f>
-        <v>0</v>
+        <v>0.0660593695372309</v>
       </c>
       <c r="E4" s="107">
         <f>IF(B4="NV",E5,B4/Einstellungen!$B$55)</f>
-        <v>0</v>
+        <v>0.00550494746143591</v>
       </c>
       <c r="K4"/>
     </row>
@@ -15296,19 +15349,19 @@
       </c>
       <c r="B5" s="105">
         <f>IF((Spezifikation!J3-(1.28*Spezifikation!M3))&lt;0,"NV",(Spezifikation!J3-(1.28*Spezifikation!M3)))</f>
-        <v>0</v>
+        <v>11.2044794406124</v>
       </c>
       <c r="C5" s="106">
         <f>IF(B5="NV",C6,B5/Einstellungen!$B$53)</f>
-        <v>0</v>
+        <v>1.40055993007656</v>
       </c>
       <c r="D5" s="106">
         <f>IF(B5="NV",D6,B5/Einstellungen!$B$54)</f>
-        <v>0</v>
+        <v>0.0700279965038278</v>
       </c>
       <c r="E5" s="107">
         <f>IF(B5="NV",E6,B5/Einstellungen!$B$55)</f>
-        <v>0</v>
+        <v>0.00583566637531898</v>
       </c>
       <c r="K5"/>
     </row>
@@ -15318,19 +15371,19 @@
       </c>
       <c r="B6" s="106">
         <f>IF((Spezifikation!J3-(1*Spezifikation!M3))&lt;0,"NV",(Spezifikation!J3-(1*Spezifikation!M3)))</f>
-        <v>0</v>
+        <v>11.4514162296451</v>
       </c>
       <c r="C6" s="106">
         <f>IF(B6="NV",C7,B6/Einstellungen!$B$53)</f>
-        <v>0</v>
+        <v>1.43142702870564</v>
       </c>
       <c r="D6" s="106">
         <f>IF(B6="NV",D7,B6/Einstellungen!$B$54)</f>
-        <v>0</v>
+        <v>0.0715713514352821</v>
       </c>
       <c r="E6" s="107">
         <f>IF(B6="NV",E7,B6/Einstellungen!$B$55)</f>
-        <v>0</v>
+        <v>0.00596427928627351</v>
       </c>
       <c r="K6"/>
     </row>
@@ -15340,19 +15393,19 @@
       </c>
       <c r="B7" s="106">
         <f>IF((Spezifikation!J3-(0.84*Spezifikation!M3))&lt;0,"NV",(Spezifikation!J3-(0.84*Spezifikation!M3)))</f>
-        <v>0</v>
+        <v>11.5925229662352</v>
       </c>
       <c r="C7" s="106">
         <f>IF(B7="NV",C8,B7/Einstellungen!$B$53)</f>
-        <v>0</v>
+        <v>1.44906537077941</v>
       </c>
       <c r="D7" s="106">
         <f>IF(B7="NV",D8,B7/Einstellungen!$B$54)</f>
-        <v>0</v>
+        <v>0.0724532685389703</v>
       </c>
       <c r="E7" s="107">
         <f>IF(B7="NV",E8,B7/Einstellungen!$B$55)</f>
-        <v>0</v>
+        <v>0.00603777237824753</v>
       </c>
       <c r="K7"/>
     </row>
@@ -15362,19 +15415,19 @@
       </c>
       <c r="B8" s="110">
         <f>IF((Spezifikation!J3-(0.67*Spezifikation!M3))&lt;0,"NV",(Spezifikation!J3-(0.67*Spezifikation!M3)))</f>
-        <v>0</v>
+        <v>11.7424488738622</v>
       </c>
       <c r="C8" s="110">
         <f>IF(B8="NV",C9,B8/Einstellungen!$B$53)</f>
-        <v>0</v>
+        <v>1.46780610923278</v>
       </c>
       <c r="D8" s="110">
         <f>IF(B8="NV",D9,B8/Einstellungen!$B$54)</f>
-        <v>0</v>
+        <v>0.073390305461639</v>
       </c>
       <c r="E8" s="110">
         <f>IF(B8="NV",E9,B8/Einstellungen!$B$55)</f>
-        <v>0</v>
+        <v>0.00611585878846992</v>
       </c>
       <c r="K8"/>
     </row>
@@ -15384,19 +15437,19 @@
       </c>
       <c r="B9" s="106">
         <f>IF((Spezifikation!J3-(0.52*Spezifikation!M3))&lt;0,"NV",(Spezifikation!J3-(0.52*Spezifikation!M3)))</f>
-        <v>0</v>
+        <v>11.8747364394155</v>
       </c>
       <c r="C9" s="106">
         <f>IF(B9="NV",C10,B9/Einstellungen!$B$53)</f>
-        <v>0</v>
+        <v>1.48434205492693</v>
       </c>
       <c r="D9" s="106">
         <f>IF(B9="NV",D10,B9/Einstellungen!$B$54)</f>
-        <v>0</v>
+        <v>0.0742171027463467</v>
       </c>
       <c r="E9" s="107">
         <f>IF(B9="NV",E10,B9/Einstellungen!$B$55)</f>
-        <v>0</v>
+        <v>0.00618475856219556</v>
       </c>
       <c r="K9"/>
     </row>
@@ -15406,19 +15459,19 @@
       </c>
       <c r="B10" s="106">
         <f>IF((Spezifikation!J3-(0.25*Spezifikation!M3))&lt;0,"NV",(Spezifikation!J3-(0.25*Spezifikation!M3)))</f>
-        <v>0</v>
+        <v>12.1128540574113</v>
       </c>
       <c r="C10" s="106">
         <f>IF(B10="NV",C11,B10/Einstellungen!$B$53)</f>
-        <v>0</v>
+        <v>1.51410675717641</v>
       </c>
       <c r="D10" s="106">
         <f>IF(B10="NV",D11,B10/Einstellungen!$B$54)</f>
-        <v>0</v>
+        <v>0.0757053378588205</v>
       </c>
       <c r="E10" s="107">
         <f>IF(B10="NV",E11,B10/Einstellungen!$B$55)</f>
-        <v>0</v>
+        <v>0.00630877815490171</v>
       </c>
       <c r="K10"/>
     </row>
@@ -15428,19 +15481,19 @@
       </c>
       <c r="B11" s="110">
         <f>Spezifikation!J3</f>
-        <v>0</v>
+        <v>12.3333333333333</v>
       </c>
       <c r="C11" s="110">
         <f>B11/Einstellungen!B53</f>
-        <v>0</v>
+        <v>1.54166666666667</v>
       </c>
       <c r="D11" s="110">
         <f>B11/Einstellungen!B54</f>
-        <v>0</v>
+        <v>0.0770833333333333</v>
       </c>
       <c r="E11" s="111">
         <f>B11/Einstellungen!B55</f>
-        <v>0</v>
+        <v>0.00642361111111111</v>
       </c>
       <c r="K11"/>
     </row>
@@ -15450,19 +15503,19 @@
       </c>
       <c r="B12" s="106">
         <f>Spezifikation!J3+(0.25*Spezifikation!M3)</f>
-        <v>0</v>
+        <v>12.5538126092554</v>
       </c>
       <c r="C12" s="106">
         <f>B12/Einstellungen!B53</f>
-        <v>0</v>
+        <v>1.56922657615692</v>
       </c>
       <c r="D12" s="106">
         <f>B12/Einstellungen!B54</f>
-        <v>0</v>
+        <v>0.0784613288078461</v>
       </c>
       <c r="E12" s="107">
         <f>B12/Einstellungen!B55</f>
-        <v>0</v>
+        <v>0.00653844406732051</v>
       </c>
       <c r="K12"/>
     </row>
@@ -15472,19 +15525,19 @@
       </c>
       <c r="B13" s="106">
         <f>Spezifikation!J3+(0.52*Spezifikation!M3)</f>
-        <v>0</v>
+        <v>12.7919302272512</v>
       </c>
       <c r="C13" s="106">
         <f>B13/Einstellungen!B53</f>
-        <v>0</v>
+        <v>1.5989912784064</v>
       </c>
       <c r="D13" s="106">
         <f>B13/Einstellungen!B54</f>
-        <v>0</v>
+        <v>0.07994956392032</v>
       </c>
       <c r="E13" s="107">
         <f>B13/Einstellungen!B55</f>
-        <v>0</v>
+        <v>0.00666246366002666</v>
       </c>
       <c r="K13"/>
     </row>
@@ -15494,19 +15547,19 @@
       </c>
       <c r="B14" s="110">
         <f>Spezifikation!J3+(0.67*Spezifikation!M3)</f>
-        <v>0</v>
+        <v>12.9242177928044</v>
       </c>
       <c r="C14" s="110">
         <f>B14/Einstellungen!B53</f>
-        <v>0</v>
+        <v>1.61552722410055</v>
       </c>
       <c r="D14" s="110">
         <f>B14/Einstellungen!B54</f>
-        <v>0</v>
+        <v>0.0807763612050277</v>
       </c>
       <c r="E14" s="111">
         <f>B14/Einstellungen!B55</f>
-        <v>0</v>
+        <v>0.0067313634337523</v>
       </c>
       <c r="K14"/>
     </row>
@@ -15516,19 +15569,19 @@
       </c>
       <c r="B15" s="106">
         <f>Spezifikation!J3+(0.84*Spezifikation!M3)</f>
-        <v>0</v>
+        <v>13.0741437004314</v>
       </c>
       <c r="C15" s="106">
         <f>B15/Einstellungen!B53</f>
-        <v>0</v>
+        <v>1.63426796255393</v>
       </c>
       <c r="D15" s="106">
         <f>B15/Einstellungen!B54</f>
-        <v>0</v>
+        <v>0.0817133981276964</v>
       </c>
       <c r="E15" s="107">
         <f>B15/Einstellungen!B55</f>
-        <v>0</v>
+        <v>0.0068094498439747</v>
       </c>
       <c r="K15"/>
     </row>
@@ -15538,19 +15591,19 @@
       </c>
       <c r="B16" s="106">
         <f>Spezifikation!J3+(1*Spezifikation!M3)</f>
-        <v>0</v>
+        <v>13.2152504370215</v>
       </c>
       <c r="C16" s="106">
         <f>B16/Einstellungen!B53</f>
-        <v>0</v>
+        <v>1.65190630462769</v>
       </c>
       <c r="D16" s="106">
         <f>B16/Einstellungen!B54</f>
-        <v>0</v>
+        <v>0.0825953152313846</v>
       </c>
       <c r="E16" s="107">
         <f>B16/Einstellungen!B55</f>
-        <v>0</v>
+        <v>0.00688294293594871</v>
       </c>
       <c r="K16"/>
     </row>
@@ -15560,19 +15613,19 @@
       </c>
       <c r="B17" s="106">
         <f>Spezifikation!J3+(1.28*Spezifikation!M3)</f>
-        <v>0</v>
+        <v>13.4621872260542</v>
       </c>
       <c r="C17" s="106">
         <f>B17/Einstellungen!B53</f>
-        <v>0</v>
+        <v>1.68277340325678</v>
       </c>
       <c r="D17" s="106">
         <f>B17/Einstellungen!B54</f>
-        <v>0</v>
+        <v>0.0841386701628389</v>
       </c>
       <c r="E17" s="107">
         <f>B17/Einstellungen!B55</f>
-        <v>0</v>
+        <v>0.00701155584690324</v>
       </c>
       <c r="K17"/>
     </row>
@@ -15582,19 +15635,19 @@
       </c>
       <c r="B18" s="113">
         <f>Spezifikation!J3+(2*Spezifikation!M3)</f>
-        <v>0</v>
+        <v>14.0971675407097</v>
       </c>
       <c r="C18" s="113">
         <f>B18/Einstellungen!B53</f>
-        <v>0</v>
+        <v>1.76214594258872</v>
       </c>
       <c r="D18" s="113">
         <f>B18/Einstellungen!B54</f>
-        <v>0</v>
+        <v>0.0881072971294358</v>
       </c>
       <c r="E18" s="114">
         <f>B18/Einstellungen!B55</f>
-        <v>0</v>
+        <v>0.00734227476078632</v>
       </c>
       <c r="K18"/>
     </row>
@@ -15625,7 +15678,7 @@
   <dimension ref="A1:F31"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F15" sqref="F15"/>
+      <selection activeCell="E8" sqref="E8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.13888888888889" defaultRowHeight="13.2" outlineLevelCol="5"/>
@@ -15640,7 +15693,7 @@
   <sheetData>
     <row r="1" ht="27" customHeight="1" spans="2:6">
       <c r="B1" s="56" t="s">
-        <v>37</v>
+        <v>43</v>
       </c>
       <c r="C1" s="56"/>
       <c r="D1" s="56"/>
@@ -15649,13 +15702,13 @@
     </row>
     <row r="2" ht="13.95" spans="2:2">
       <c r="B2" s="57" t="s">
-        <v>38</v>
+        <v>44</v>
       </c>
     </row>
     <row r="3" s="54" customFormat="1" ht="33.75" customHeight="1" spans="1:6">
       <c r="A3" s="58"/>
       <c r="B3" s="59" t="s">
-        <v>39</v>
+        <v>45</v>
       </c>
       <c r="C3" s="60"/>
       <c r="F3" s="61"/>
@@ -15668,7 +15721,7 @@
     <row r="5" ht="13.8" spans="1:3">
       <c r="A5" s="62"/>
       <c r="B5" s="65" t="s">
-        <v>40</v>
+        <v>46</v>
       </c>
       <c r="C5" s="66">
         <v>139</v>
@@ -15677,7 +15730,7 @@
     <row r="6" ht="13.8" spans="1:3">
       <c r="A6" s="62"/>
       <c r="B6" s="65" t="s">
-        <v>41</v>
+        <v>47</v>
       </c>
       <c r="C6" s="66">
         <v>7.7</v>
@@ -15686,7 +15739,7 @@
     <row r="7" ht="14.55" spans="1:3">
       <c r="A7" s="62"/>
       <c r="B7" s="67" t="s">
-        <v>42</v>
+        <v>48</v>
       </c>
       <c r="C7" s="68">
         <f>C5*C6</f>
@@ -15696,14 +15749,14 @@
     <row r="8" spans="1:3">
       <c r="A8" s="62"/>
       <c r="B8" s="69" t="s">
-        <v>43</v>
+        <v>49</v>
       </c>
       <c r="C8" s="70"/>
     </row>
     <row r="9" spans="1:3">
       <c r="A9" s="62"/>
       <c r="B9" s="69" t="s">
-        <v>44</v>
+        <v>50</v>
       </c>
       <c r="C9" s="70"/>
     </row>
@@ -15720,7 +15773,7 @@
     </row>
     <row r="12" ht="13.95" spans="2:4">
       <c r="B12" s="73" t="s">
-        <v>45</v>
+        <v>51</v>
       </c>
       <c r="C12" s="72"/>
       <c r="D12" s="72"/>
@@ -15729,66 +15782,66 @@
       <c r="A13" s="62"/>
       <c r="B13" s="59"/>
       <c r="C13" s="74" t="s">
-        <v>46</v>
+        <v>52</v>
       </c>
       <c r="D13" s="75" t="s">
-        <v>47</v>
+        <v>53</v>
       </c>
       <c r="E13" s="74" t="s">
-        <v>48</v>
+        <v>54</v>
       </c>
       <c r="F13" s="76" t="s">
-        <v>49</v>
+        <v>55</v>
       </c>
     </row>
     <row r="14" spans="1:6">
       <c r="A14" s="62"/>
       <c r="B14" s="65" t="s">
-        <v>50</v>
+        <v>56</v>
       </c>
       <c r="C14" s="77">
         <f>Aufwandschätzung!B8</f>
-        <v>0</v>
+        <v>11.7424488738622</v>
       </c>
       <c r="D14" s="77">
         <f>Aufwandschätzung!B11</f>
-        <v>0</v>
+        <v>12.3333333333333</v>
       </c>
       <c r="E14" s="77">
         <f>Aufwandschätzung!B14</f>
-        <v>0</v>
+        <v>12.9242177928044</v>
       </c>
       <c r="F14" s="78">
         <f>Aufwandschätzung!B18</f>
-        <v>0</v>
+        <v>14.0971675407097</v>
       </c>
     </row>
     <row r="15" spans="1:6">
       <c r="A15" s="62"/>
       <c r="B15" s="65" t="s">
-        <v>51</v>
+        <v>57</v>
       </c>
       <c r="C15" s="79">
         <f>C14/C6</f>
-        <v>0</v>
+        <v>1.52499336024185</v>
       </c>
       <c r="D15" s="79">
         <f>D14/C6</f>
-        <v>0</v>
+        <v>1.6017316017316</v>
       </c>
       <c r="E15" s="79">
         <f>E14/C6</f>
-        <v>0</v>
+        <v>1.67846984322135</v>
       </c>
       <c r="F15" s="80">
         <f>F14/C6</f>
-        <v>0</v>
+        <v>1.83080097931295</v>
       </c>
     </row>
     <row r="16" spans="1:6">
       <c r="A16" s="62"/>
       <c r="B16" s="65" t="s">
-        <v>52</v>
+        <v>58</v>
       </c>
       <c r="C16" s="81">
         <v>0</v>
@@ -15806,7 +15859,7 @@
     <row r="17" spans="1:6">
       <c r="A17" s="62"/>
       <c r="B17" s="65" t="s">
-        <v>53</v>
+        <v>59</v>
       </c>
       <c r="C17" s="81">
         <v>0</v>
@@ -15832,41 +15885,41 @@
     <row r="19" spans="1:6">
       <c r="A19" s="62"/>
       <c r="B19" s="65" t="s">
-        <v>54</v>
+        <v>60</v>
       </c>
       <c r="C19" s="83">
         <f>(C5*C14)+C16+C17</f>
-        <v>0</v>
+        <v>1632.20039346685</v>
       </c>
       <c r="D19" s="83">
         <f>(C5*D14)+D16+D17</f>
-        <v>0</v>
+        <v>1714.33333333333</v>
       </c>
       <c r="E19" s="83">
         <f>(C5*E14)+E16+E17</f>
-        <v>0</v>
+        <v>1796.46627319982</v>
       </c>
       <c r="F19" s="86">
         <f>(C5*F14)+F16+F17</f>
-        <v>0</v>
+        <v>1959.50628815865</v>
       </c>
     </row>
     <row r="20" ht="53.55" spans="1:6">
       <c r="A20" s="62"/>
       <c r="B20" s="87" t="s">
-        <v>55</v>
+        <v>61</v>
       </c>
       <c r="C20" s="88" t="s">
-        <v>56</v>
+        <v>62</v>
       </c>
       <c r="D20" s="88" t="s">
-        <v>57</v>
+        <v>63</v>
       </c>
       <c r="E20" s="88" t="s">
-        <v>58</v>
+        <v>64</v>
       </c>
       <c r="F20" s="89" t="s">
-        <v>59</v>
+        <v>65</v>
       </c>
     </row>
     <row r="21" spans="1:4">
@@ -15954,7 +16007,7 @@
   <sheetData>
     <row r="1" ht="15.15" spans="1:7">
       <c r="A1" s="2" t="s">
-        <v>60</v>
+        <v>66</v>
       </c>
       <c r="B1" s="3"/>
       <c r="C1" s="3"/>
@@ -15965,163 +16018,163 @@
     </row>
     <row r="2" ht="29.55" spans="1:7">
       <c r="A2" s="4" t="s">
-        <v>61</v>
+        <v>67</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>62</v>
+        <v>68</v>
       </c>
       <c r="C2" s="5" t="s">
-        <v>63</v>
+        <v>69</v>
       </c>
       <c r="D2" s="5" t="s">
-        <v>64</v>
+        <v>70</v>
       </c>
       <c r="E2" s="5" t="s">
-        <v>65</v>
+        <v>71</v>
       </c>
       <c r="F2" s="5" t="s">
-        <v>66</v>
+        <v>72</v>
       </c>
       <c r="G2" s="6" t="s">
-        <v>67</v>
+        <v>73</v>
       </c>
     </row>
     <row r="3" ht="14.4" spans="1:7">
       <c r="A3" s="7" t="s">
-        <v>62</v>
+        <v>68</v>
       </c>
       <c r="B3" s="8" t="s">
-        <v>62</v>
+        <v>68</v>
       </c>
       <c r="C3" s="8" t="s">
-        <v>63</v>
+        <v>69</v>
       </c>
       <c r="D3" s="8" t="s">
-        <v>64</v>
+        <v>70</v>
       </c>
       <c r="E3" s="8" t="s">
-        <v>65</v>
+        <v>71</v>
       </c>
       <c r="F3" s="8" t="s">
-        <v>66</v>
+        <v>72</v>
       </c>
       <c r="G3" s="9" t="s">
-        <v>67</v>
+        <v>73</v>
       </c>
     </row>
     <row r="4" ht="14.4" spans="1:7">
       <c r="A4" s="7" t="s">
-        <v>63</v>
+        <v>69</v>
       </c>
       <c r="B4" s="8" t="s">
-        <v>62</v>
+        <v>68</v>
       </c>
       <c r="C4" s="8" t="s">
-        <v>63</v>
+        <v>69</v>
       </c>
       <c r="D4" s="8" t="s">
-        <v>64</v>
+        <v>70</v>
       </c>
       <c r="E4" s="8" t="s">
-        <v>65</v>
+        <v>71</v>
       </c>
       <c r="F4" s="8" t="s">
-        <v>66</v>
+        <v>72</v>
       </c>
       <c r="G4" s="9" t="s">
-        <v>67</v>
+        <v>73</v>
       </c>
     </row>
     <row r="5" ht="14.4" spans="1:7">
       <c r="A5" s="7" t="s">
-        <v>64</v>
+        <v>70</v>
       </c>
       <c r="B5" s="8" t="s">
-        <v>62</v>
+        <v>68</v>
       </c>
       <c r="C5" s="8" t="s">
-        <v>62</v>
+        <v>68</v>
       </c>
       <c r="D5" s="8" t="s">
-        <v>64</v>
+        <v>70</v>
       </c>
       <c r="E5" s="8" t="s">
-        <v>65</v>
+        <v>71</v>
       </c>
       <c r="F5" s="8" t="s">
-        <v>66</v>
+        <v>72</v>
       </c>
       <c r="G5" s="9" t="s">
-        <v>67</v>
+        <v>73</v>
       </c>
     </row>
     <row r="6" ht="14.4" spans="1:7">
       <c r="A6" s="7" t="s">
-        <v>65</v>
+        <v>71</v>
       </c>
       <c r="B6" s="8" t="s">
-        <v>62</v>
+        <v>68</v>
       </c>
       <c r="C6" s="8" t="s">
-        <v>62</v>
+        <v>68</v>
       </c>
       <c r="D6" s="8" t="s">
-        <v>63</v>
+        <v>69</v>
       </c>
       <c r="E6" s="8" t="s">
-        <v>65</v>
+        <v>71</v>
       </c>
       <c r="F6" s="8" t="s">
-        <v>66</v>
+        <v>72</v>
       </c>
       <c r="G6" s="9" t="s">
-        <v>67</v>
+        <v>73</v>
       </c>
     </row>
     <row r="7" ht="14.4" spans="1:7">
       <c r="A7" s="7" t="s">
-        <v>66</v>
+        <v>72</v>
       </c>
       <c r="B7" s="8" t="s">
-        <v>62</v>
+        <v>68</v>
       </c>
       <c r="C7" s="8" t="s">
-        <v>62</v>
+        <v>68</v>
       </c>
       <c r="D7" s="8" t="s">
-        <v>63</v>
+        <v>69</v>
       </c>
       <c r="E7" s="8" t="s">
-        <v>64</v>
+        <v>70</v>
       </c>
       <c r="F7" s="8" t="s">
-        <v>66</v>
+        <v>72</v>
       </c>
       <c r="G7" s="9" t="s">
-        <v>67</v>
+        <v>73</v>
       </c>
     </row>
     <row r="8" ht="15.15" spans="1:7">
       <c r="A8" s="10" t="s">
-        <v>67</v>
+        <v>73</v>
       </c>
       <c r="B8" s="11" t="s">
-        <v>62</v>
+        <v>68</v>
       </c>
       <c r="C8" s="11" t="s">
-        <v>62</v>
+        <v>68</v>
       </c>
       <c r="D8" s="11" t="s">
-        <v>63</v>
+        <v>69</v>
       </c>
       <c r="E8" s="11" t="s">
-        <v>64</v>
+        <v>70</v>
       </c>
       <c r="F8" s="11" t="s">
-        <v>65</v>
+        <v>71</v>
       </c>
       <c r="G8" s="12" t="s">
-        <v>67</v>
+        <v>73</v>
       </c>
     </row>
     <row r="9" ht="14.4" spans="1:7">
@@ -16135,13 +16188,13 @@
     </row>
     <row r="10" ht="14.4" spans="1:7">
       <c r="A10" s="14" t="s">
-        <v>60</v>
+        <v>66</v>
       </c>
       <c r="B10" s="14" t="s">
-        <v>68</v>
+        <v>74</v>
       </c>
       <c r="C10" s="14" t="s">
-        <v>69</v>
+        <v>75</v>
       </c>
       <c r="D10" s="3"/>
       <c r="E10" s="3"/>
@@ -16150,13 +16203,13 @@
     </row>
     <row r="11" ht="14.4" spans="1:7">
       <c r="A11" s="14" t="s">
-        <v>62</v>
+        <v>68</v>
       </c>
       <c r="B11" s="13" t="s">
-        <v>70</v>
+        <v>76</v>
       </c>
       <c r="C11" s="13" t="s">
-        <v>70</v>
+        <v>76</v>
       </c>
       <c r="D11" s="3"/>
       <c r="E11" s="3"/>
@@ -16165,13 +16218,13 @@
     </row>
     <row r="12" ht="14.4" spans="1:7">
       <c r="A12" s="14" t="s">
-        <v>63</v>
+        <v>69</v>
       </c>
       <c r="B12" s="13" t="s">
-        <v>71</v>
+        <v>77</v>
       </c>
       <c r="C12" s="13" t="s">
-        <v>70</v>
+        <v>76</v>
       </c>
       <c r="D12" s="3"/>
       <c r="E12" s="3"/>
@@ -16180,13 +16233,13 @@
     </row>
     <row r="13" ht="14.4" spans="1:7">
       <c r="A13" s="14" t="s">
-        <v>64</v>
+        <v>70</v>
       </c>
       <c r="B13" s="13" t="s">
-        <v>72</v>
+        <v>78</v>
       </c>
       <c r="C13" s="13" t="s">
-        <v>70</v>
+        <v>76</v>
       </c>
       <c r="D13" s="3"/>
       <c r="E13" s="3"/>
@@ -16195,13 +16248,13 @@
     </row>
     <row r="14" ht="14.4" spans="1:7">
       <c r="A14" s="14" t="s">
-        <v>65</v>
+        <v>71</v>
       </c>
       <c r="B14" s="13" t="s">
-        <v>73</v>
+        <v>79</v>
       </c>
       <c r="C14" s="3" t="s">
-        <v>74</v>
+        <v>80</v>
       </c>
       <c r="D14" s="3"/>
       <c r="E14" s="3"/>
@@ -16210,13 +16263,13 @@
     </row>
     <row r="15" ht="14.4" spans="1:7">
       <c r="A15" s="14" t="s">
-        <v>66</v>
+        <v>72</v>
       </c>
       <c r="B15" s="3" t="s">
-        <v>75</v>
+        <v>81</v>
       </c>
       <c r="C15" s="3" t="s">
-        <v>74</v>
+        <v>80</v>
       </c>
       <c r="D15" s="3"/>
       <c r="E15" s="3"/>
@@ -16225,13 +16278,13 @@
     </row>
     <row r="16" ht="14.4" spans="1:7">
       <c r="A16" s="14" t="s">
-        <v>67</v>
+        <v>73</v>
       </c>
       <c r="B16" s="3" t="s">
-        <v>76</v>
+        <v>82</v>
       </c>
       <c r="C16" s="3" t="s">
-        <v>74</v>
+        <v>80</v>
       </c>
       <c r="D16" s="3"/>
       <c r="E16" s="3"/>
@@ -16249,31 +16302,31 @@
     </row>
     <row r="19" ht="14.4" spans="1:1">
       <c r="A19" s="14" t="s">
-        <v>77</v>
+        <v>83</v>
       </c>
     </row>
     <row r="20" ht="13.95"/>
     <row r="21" ht="39" customHeight="1" spans="1:7">
       <c r="A21" s="15" t="s">
-        <v>78</v>
+        <v>84</v>
       </c>
       <c r="B21" s="16" t="s">
-        <v>79</v>
+        <v>85</v>
       </c>
       <c r="C21" s="16" t="s">
-        <v>80</v>
+        <v>86</v>
       </c>
       <c r="D21" s="16" t="s">
-        <v>81</v>
+        <v>87</v>
       </c>
       <c r="E21" s="16" t="s">
-        <v>82</v>
+        <v>88</v>
       </c>
       <c r="F21" s="16" t="s">
-        <v>83</v>
+        <v>89</v>
       </c>
       <c r="G21" s="17" t="s">
-        <v>84</v>
+        <v>90</v>
       </c>
     </row>
     <row r="22" spans="1:7">
@@ -16285,7 +16338,7 @@
         <v>512</v>
       </c>
       <c r="C22" s="20" t="s">
-        <v>67</v>
+        <v>73</v>
       </c>
       <c r="D22" s="21">
         <f t="shared" ref="D22:D33" si="1">(A22*storypoints_kalibrierung)/8</f>
@@ -16296,10 +16349,10 @@
         <v>3.2</v>
       </c>
       <c r="F22" s="22" t="s">
-        <v>85</v>
+        <v>91</v>
       </c>
       <c r="G22" s="23" t="s">
-        <v>86</v>
+        <v>92</v>
       </c>
     </row>
     <row r="23" spans="1:7">
@@ -16311,7 +16364,7 @@
         <v>256</v>
       </c>
       <c r="C23" s="20" t="s">
-        <v>67</v>
+        <v>73</v>
       </c>
       <c r="D23" s="21">
         <f t="shared" si="1"/>
@@ -16322,10 +16375,10 @@
         <v>1.6</v>
       </c>
       <c r="F23" s="22" t="s">
-        <v>85</v>
+        <v>91</v>
       </c>
       <c r="G23" s="23" t="s">
-        <v>86</v>
+        <v>92</v>
       </c>
     </row>
     <row r="24" spans="1:7">
@@ -16337,7 +16390,7 @@
         <v>128</v>
       </c>
       <c r="C24" s="24" t="s">
-        <v>67</v>
+        <v>73</v>
       </c>
       <c r="D24" s="21">
         <f t="shared" si="1"/>
@@ -16348,10 +16401,10 @@
         <v>0.8</v>
       </c>
       <c r="F24" s="22" t="s">
-        <v>85</v>
+        <v>91</v>
       </c>
       <c r="G24" s="23" t="s">
-        <v>86</v>
+        <v>92</v>
       </c>
     </row>
     <row r="25" spans="1:7">
@@ -16363,7 +16416,7 @@
         <v>64</v>
       </c>
       <c r="C25" s="24" t="s">
-        <v>66</v>
+        <v>72</v>
       </c>
       <c r="D25" s="21">
         <f t="shared" si="1"/>
@@ -16374,10 +16427,10 @@
         <v>0.4</v>
       </c>
       <c r="F25" s="22" t="s">
-        <v>85</v>
+        <v>91</v>
       </c>
       <c r="G25" s="23" t="s">
-        <v>86</v>
+        <v>92</v>
       </c>
     </row>
     <row r="26" spans="1:7">
@@ -16389,7 +16442,7 @@
         <v>32</v>
       </c>
       <c r="C26" s="20" t="s">
-        <v>65</v>
+        <v>71</v>
       </c>
       <c r="D26" s="21">
         <f t="shared" si="1"/>
@@ -16400,10 +16453,10 @@
         <v>0.2</v>
       </c>
       <c r="F26" s="22" t="s">
-        <v>87</v>
+        <v>93</v>
       </c>
       <c r="G26" s="23" t="s">
-        <v>88</v>
+        <v>94</v>
       </c>
     </row>
     <row r="27" spans="1:7">
@@ -16415,7 +16468,7 @@
         <v>16</v>
       </c>
       <c r="C27" s="20" t="s">
-        <v>65</v>
+        <v>71</v>
       </c>
       <c r="D27" s="21">
         <f t="shared" si="1"/>
@@ -16426,10 +16479,10 @@
         <v>0.1</v>
       </c>
       <c r="F27" s="25" t="s">
-        <v>89</v>
+        <v>95</v>
       </c>
       <c r="G27" s="26" t="s">
-        <v>90</v>
+        <v>96</v>
       </c>
     </row>
     <row r="28" spans="1:7">
@@ -16441,7 +16494,7 @@
         <v>8</v>
       </c>
       <c r="C28" s="20" t="s">
-        <v>64</v>
+        <v>70</v>
       </c>
       <c r="D28" s="21">
         <f t="shared" si="1"/>
@@ -16452,10 +16505,10 @@
         <v>0.05</v>
       </c>
       <c r="F28" s="25" t="s">
-        <v>89</v>
+        <v>95</v>
       </c>
       <c r="G28" s="26" t="s">
-        <v>91</v>
+        <v>97</v>
       </c>
     </row>
     <row r="29" spans="1:7">
@@ -16467,7 +16520,7 @@
         <v>4</v>
       </c>
       <c r="C29" s="20" t="s">
-        <v>64</v>
+        <v>70</v>
       </c>
       <c r="D29" s="21">
         <f t="shared" si="1"/>
@@ -16478,10 +16531,10 @@
         <v>0.025</v>
       </c>
       <c r="F29" s="25" t="s">
-        <v>89</v>
+        <v>95</v>
       </c>
       <c r="G29" s="23" t="s">
-        <v>91</v>
+        <v>97</v>
       </c>
     </row>
     <row r="30" spans="1:7">
@@ -16493,7 +16546,7 @@
         <v>2</v>
       </c>
       <c r="C30" s="20" t="s">
-        <v>63</v>
+        <v>69</v>
       </c>
       <c r="D30" s="21">
         <f t="shared" si="1"/>
@@ -16504,10 +16557,10 @@
         <v>0.0125</v>
       </c>
       <c r="F30" s="25" t="s">
-        <v>89</v>
+        <v>95</v>
       </c>
       <c r="G30" s="23" t="s">
-        <v>91</v>
+        <v>97</v>
       </c>
     </row>
     <row r="31" spans="1:7">
@@ -16518,7 +16571,7 @@
         <v>1</v>
       </c>
       <c r="C31" s="20" t="s">
-        <v>63</v>
+        <v>69</v>
       </c>
       <c r="D31" s="21">
         <f t="shared" si="1"/>
@@ -16529,10 +16582,10 @@
         <v>0.00625</v>
       </c>
       <c r="F31" s="29" t="s">
-        <v>89</v>
+        <v>95</v>
       </c>
       <c r="G31" s="30" t="s">
-        <v>91</v>
+        <v>97</v>
       </c>
     </row>
     <row r="32" spans="1:7">
@@ -16544,7 +16597,7 @@
         <v>0.5</v>
       </c>
       <c r="C32" s="20" t="s">
-        <v>62</v>
+        <v>68</v>
       </c>
       <c r="D32" s="21">
         <f t="shared" si="1"/>
@@ -16555,10 +16608,10 @@
         <v>0.003125</v>
       </c>
       <c r="F32" s="25" t="s">
-        <v>89</v>
+        <v>95</v>
       </c>
       <c r="G32" s="23" t="s">
-        <v>91</v>
+        <v>97</v>
       </c>
     </row>
     <row r="33" ht="13.95" spans="1:7">
@@ -16570,7 +16623,7 @@
         <v>0</v>
       </c>
       <c r="C33" s="33" t="s">
-        <v>62</v>
+        <v>68</v>
       </c>
       <c r="D33" s="34">
         <f t="shared" si="1"/>
@@ -16581,15 +16634,15 @@
         <v>0</v>
       </c>
       <c r="F33" s="35" t="s">
-        <v>89</v>
+        <v>95</v>
       </c>
       <c r="G33" s="36" t="s">
-        <v>91</v>
+        <v>97</v>
       </c>
     </row>
     <row r="35" ht="18" customHeight="1" spans="1:1">
       <c r="A35" s="37" t="s">
-        <v>92</v>
+        <v>98</v>
       </c>
     </row>
     <row r="36" ht="18" customHeight="1" spans="1:1">
@@ -16597,10 +16650,10 @@
     </row>
     <row r="37" ht="93.15" spans="1:2">
       <c r="A37" s="38" t="s">
-        <v>93</v>
+        <v>99</v>
       </c>
       <c r="B37" s="39" t="s">
-        <v>94</v>
+        <v>100</v>
       </c>
     </row>
     <row r="38" spans="1:2">
@@ -16608,7 +16661,7 @@
         <v>100</v>
       </c>
       <c r="B38" s="41" t="s">
-        <v>95</v>
+        <v>101</v>
       </c>
     </row>
     <row r="39" spans="1:2">
@@ -16701,21 +16754,21 @@
     </row>
     <row r="51" ht="13.95" spans="1:2">
       <c r="A51" s="37" t="s">
-        <v>96</v>
+        <v>102</v>
       </c>
       <c r="B51" s="46"/>
     </row>
     <row r="52" ht="26.4" spans="1:2">
       <c r="A52" s="47" t="s">
-        <v>97</v>
+        <v>103</v>
       </c>
       <c r="B52" s="48" t="s">
-        <v>98</v>
+        <v>104</v>
       </c>
     </row>
     <row r="53" spans="1:2">
       <c r="A53" s="49" t="s">
-        <v>99</v>
+        <v>105</v>
       </c>
       <c r="B53" s="50">
         <v>8</v>
@@ -16723,7 +16776,7 @@
     </row>
     <row r="54" spans="1:2">
       <c r="A54" s="49" t="s">
-        <v>100</v>
+        <v>106</v>
       </c>
       <c r="B54" s="50">
         <v>160</v>
@@ -16731,7 +16784,7 @@
     </row>
     <row r="55" ht="13.95" spans="1:2">
       <c r="A55" s="51" t="s">
-        <v>101</v>
+        <v>107</v>
       </c>
       <c r="B55" s="52">
         <f>160*12</f>
@@ -16740,7 +16793,7 @@
     </row>
     <row r="56" spans="1:1">
       <c r="A56" s="53" t="s">
-        <v>102</v>
+        <v>108</v>
       </c>
     </row>
   </sheetData>

</xml_diff>